<commit_message>
tweak analyses per reviewer requests
</commit_message>
<xml_diff>
--- a/data/demographics.xlsx
+++ b/data/demographics.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/evanmaclean/Box Sync/NIH_WALTHAM_HAI_studies/Data/analysis_ready/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19261ED0-93A4-3F4D-B78D-7B61BD9E2249}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C71C9FB-879C-104F-8C76-C60F89E490EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4560" yWindow="2080" windowWidth="28040" windowHeight="16340" xr2:uid="{10801737-9405-E04D-AFC2-336E6F5D8C40}"/>
+    <workbookView xWindow="55040" yWindow="5120" windowWidth="28040" windowHeight="16340" xr2:uid="{10801737-9405-E04D-AFC2-336E6F5D8C40}"/>
   </bookViews>
   <sheets>
     <sheet name="DogDems" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="71">
   <si>
     <t>ID</t>
   </si>
@@ -86,9 +86,6 @@
   </si>
   <si>
     <t>N</t>
-  </si>
-  <si>
-    <t>NA</t>
   </si>
   <si>
     <t>Maltipoo</t>
@@ -612,12 +609,14 @@
   <dimension ref="A1:H56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="E58" sqref="E58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="18.5" customWidth="1"/>
+    <col min="4" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.83203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="25.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="30.6640625" customWidth="1"/>
     <col min="8" max="8" width="13.5" bestFit="1" customWidth="1"/>
@@ -640,13 +639,13 @@
         <v>16</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>17</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -669,10 +668,10 @@
         <v>3</v>
       </c>
       <c r="G2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
@@ -695,10 +694,10 @@
         <v>13</v>
       </c>
       <c r="G3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -721,10 +720,10 @@
         <v>12</v>
       </c>
       <c r="G4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -747,10 +746,10 @@
         <v>3</v>
       </c>
       <c r="G5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -773,10 +772,10 @@
         <v>2</v>
       </c>
       <c r="G6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -793,16 +792,16 @@
         <v>1.5</v>
       </c>
       <c r="E7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F7">
         <v>0.42</v>
       </c>
       <c r="G7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
@@ -825,10 +824,10 @@
         <v>4.5</v>
       </c>
       <c r="G8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
@@ -851,10 +850,10 @@
         <v>5</v>
       </c>
       <c r="G9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
@@ -877,10 +876,10 @@
         <v>4</v>
       </c>
       <c r="G10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
@@ -903,10 +902,10 @@
         <v>1.5</v>
       </c>
       <c r="G11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
@@ -929,10 +928,10 @@
         <v>3</v>
       </c>
       <c r="G12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
@@ -955,10 +954,10 @@
         <v>4</v>
       </c>
       <c r="G13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
@@ -981,10 +980,10 @@
         <v>2</v>
       </c>
       <c r="G14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H14" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
@@ -1007,10 +1006,10 @@
         <v>12</v>
       </c>
       <c r="G15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
@@ -1033,10 +1032,10 @@
         <v>2</v>
       </c>
       <c r="G16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H16" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
@@ -1059,10 +1058,10 @@
         <v>0.5</v>
       </c>
       <c r="G17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
@@ -1085,10 +1084,10 @@
         <v>6</v>
       </c>
       <c r="G18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H18" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
@@ -1111,10 +1110,10 @@
         <v>1</v>
       </c>
       <c r="G19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H19" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
@@ -1137,10 +1136,10 @@
         <v>2.75</v>
       </c>
       <c r="G20" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H20" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
@@ -1163,10 +1162,10 @@
         <v>1</v>
       </c>
       <c r="G21" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H21" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
@@ -1189,10 +1188,10 @@
         <v>3</v>
       </c>
       <c r="G22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H22" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
@@ -1215,10 +1214,10 @@
         <v>3</v>
       </c>
       <c r="G23" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H23" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
@@ -1241,10 +1240,10 @@
         <v>1</v>
       </c>
       <c r="G24" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H24" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
@@ -1267,10 +1266,10 @@
         <v>0.83</v>
       </c>
       <c r="G25" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
@@ -1293,10 +1292,10 @@
         <v>11</v>
       </c>
       <c r="G26" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H26" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
@@ -1319,10 +1318,10 @@
         <v>2</v>
       </c>
       <c r="G27" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H27" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
@@ -1345,10 +1344,10 @@
         <v>0.5</v>
       </c>
       <c r="G28" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H28" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
@@ -1371,10 +1370,10 @@
         <v>6.5</v>
       </c>
       <c r="G29" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H29" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
@@ -1397,10 +1396,10 @@
         <v>8</v>
       </c>
       <c r="G30" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H30" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
@@ -1423,10 +1422,10 @@
         <v>3</v>
       </c>
       <c r="G31" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H31" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
@@ -1449,10 +1448,10 @@
         <v>3</v>
       </c>
       <c r="G32" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H32" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
@@ -1475,10 +1474,10 @@
         <v>0.57999999999999996</v>
       </c>
       <c r="G33" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H33" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
@@ -1501,10 +1500,10 @@
         <v>3.5</v>
       </c>
       <c r="G34" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H34" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
@@ -1527,10 +1526,10 @@
         <v>1</v>
       </c>
       <c r="G35" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H35" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
@@ -1553,10 +1552,10 @@
         <v>4</v>
       </c>
       <c r="G36" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H36" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
@@ -1579,10 +1578,10 @@
         <v>7</v>
       </c>
       <c r="G37" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H37" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
@@ -1605,10 +1604,10 @@
         <v>4.5</v>
       </c>
       <c r="G38" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H38" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
@@ -1631,10 +1630,10 @@
         <v>4</v>
       </c>
       <c r="G39" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H39" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
@@ -1657,10 +1656,10 @@
         <v>3</v>
       </c>
       <c r="G40" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H40" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
@@ -1683,10 +1682,10 @@
         <v>14</v>
       </c>
       <c r="G41" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H41" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
@@ -1709,10 +1708,10 @@
         <v>5</v>
       </c>
       <c r="G42" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H42" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
@@ -1735,10 +1734,10 @@
         <v>4</v>
       </c>
       <c r="G43" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H43" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
@@ -1761,10 +1760,10 @@
         <v>6</v>
       </c>
       <c r="G44" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H44" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
@@ -1787,10 +1786,10 @@
         <v>5</v>
       </c>
       <c r="G45" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H45" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
@@ -1813,10 +1812,10 @@
         <v>2</v>
       </c>
       <c r="G46" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H46" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
@@ -1839,10 +1838,10 @@
         <v>6</v>
       </c>
       <c r="G47" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H47" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
@@ -1865,10 +1864,10 @@
         <v>0.625</v>
       </c>
       <c r="G48" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H48" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
@@ -1891,10 +1890,10 @@
         <v>2</v>
       </c>
       <c r="G49" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H49" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
@@ -1917,10 +1916,10 @@
         <v>5</v>
       </c>
       <c r="G50" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H50" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
@@ -1943,10 +1942,10 @@
         <v>10</v>
       </c>
       <c r="G51" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H51" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
@@ -1969,10 +1968,10 @@
         <v>3</v>
       </c>
       <c r="G52" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H52" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
@@ -1995,10 +1994,10 @@
         <v>4.5</v>
       </c>
       <c r="G53" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H53" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
@@ -2021,10 +2020,10 @@
         <v>0.5</v>
       </c>
       <c r="G54" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H54" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
@@ -2047,10 +2046,10 @@
         <v>3</v>
       </c>
       <c r="G55" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H55" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
@@ -2073,10 +2072,10 @@
         <v>6</v>
       </c>
       <c r="G56" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H56" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -2193,7 +2192,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F5" t="s">
         <v>15</v>
@@ -2213,7 +2212,7 @@
         <v>10</v>
       </c>
       <c r="E6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F6" t="s">
         <v>15</v>
@@ -2293,7 +2292,7 @@
         <v>10</v>
       </c>
       <c r="E10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F10" t="s">
         <v>14</v>
@@ -2373,7 +2372,7 @@
         <v>10</v>
       </c>
       <c r="E14" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F14" t="s">
         <v>15</v>
@@ -2953,7 +2952,7 @@
         <v>10</v>
       </c>
       <c r="E43" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F43" t="s">
         <v>14</v>
@@ -2993,7 +2992,7 @@
         <v>10</v>
       </c>
       <c r="E45" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F45" t="s">
         <v>14</v>
@@ -3093,7 +3092,7 @@
         <v>10</v>
       </c>
       <c r="E50" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F50" t="s">
         <v>14</v>
@@ -3173,7 +3172,7 @@
         <v>10</v>
       </c>
       <c r="E54" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F54" t="s">
         <v>14</v>

</xml_diff>